<commit_message>
atualização da lista de materiais
</commit_message>
<xml_diff>
--- a/Materiais.xlsx
+++ b/Materiais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\GitHub\Prusa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571A5A27-548B-4EBC-A215-EF8A5046ED54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C652E6-F810-405B-B82F-0EB1AD496CC1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{AE9EF232-B713-46EB-8C7C-A8B1241BBC5C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="60">
   <si>
     <t>Peça</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>falta definir comprimento</t>
+  </si>
+  <si>
+    <t>3 peças, falta botão stopper</t>
+  </si>
+  <si>
+    <t>parafuso CHC M5x47</t>
+  </si>
+  <si>
+    <t>para carro da cama quente</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -404,6 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4442A1-F99D-40F7-B3FB-0F573F96FE29}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1385,10 @@
         <v>11</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1408,6 +1421,43 @@
       <c r="G33" s="1" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
atualização de lista de peças
</commit_message>
<xml_diff>
--- a/Materiais.xlsx
+++ b/Materiais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\GitHub\Prusa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C652E6-F810-405B-B82F-0EB1AD496CC1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416B4145-DF3C-4727-B431-E391F8AD72FD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{AE9EF232-B713-46EB-8C7C-A8B1241BBC5C}"/>
   </bookViews>
@@ -404,6 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,7 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4442A1-F99D-40F7-B3FB-0F573F96FE29}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,14 +799,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
       <c r="J1" t="s">
         <v>2</v>
       </c>
@@ -864,7 +864,7 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>17</v>
@@ -937,7 +937,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>17</v>
@@ -954,7 +954,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>17</v>
@@ -1060,7 +1060,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>13</v>
@@ -1080,7 +1080,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>51</v>
@@ -1120,7 +1120,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
         <v>8</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>13</v>
@@ -1256,7 +1256,7 @@
         <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>17</v>
@@ -1350,7 +1350,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1385,7 +1385,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>57</v>
@@ -1457,7 +1457,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F37" s="22"/>
+      <c r="F37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
alterações a peças para imprimir
</commit_message>
<xml_diff>
--- a/Materiais.xlsx
+++ b/Materiais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\GitHub\Prusa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416B4145-DF3C-4727-B431-E391F8AD72FD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F58DF89-C90A-4374-9C76-EB928FF549A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{AE9EF232-B713-46EB-8C7C-A8B1241BBC5C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="60">
   <si>
     <t>Peça</t>
   </si>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4442A1-F99D-40F7-B3FB-0F573F96FE29}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,13 +891,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -917,7 +914,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>17</v>
@@ -1025,7 +1022,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>50</v>
@@ -1042,13 +1039,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="J12" s="15"/>
     </row>
@@ -1242,7 +1236,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update da lista de peças
</commit_message>
<xml_diff>
--- a/Materiais.xlsx
+++ b/Materiais.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\GitHub\Prusa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F58DF89-C90A-4374-9C76-EB928FF549A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5EDC89-4C7E-40AD-A5F2-025884850043}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{AE9EF232-B713-46EB-8C7C-A8B1241BBC5C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
   <si>
     <t>Peça</t>
   </si>
@@ -189,9 +189,6 @@
     <t>carro para cama quente</t>
   </si>
   <si>
-    <t>parafuso CHC M4x38</t>
-  </si>
-  <si>
     <t>parafuso CHC M3x</t>
   </si>
   <si>
@@ -201,10 +198,25 @@
     <t>3 peças, falta botão stopper</t>
   </si>
   <si>
-    <t>parafuso CHC M5x47</t>
-  </si>
-  <si>
     <t>para carro da cama quente</t>
+  </si>
+  <si>
+    <t>parafuso CHC M4x40</t>
+  </si>
+  <si>
+    <t>parafuso CHC M3x12</t>
+  </si>
+  <si>
+    <t>parafuso CHC M5x50</t>
+  </si>
+  <si>
+    <t>parafuso CHC M5x35</t>
+  </si>
+  <si>
+    <t>parafuso CHC M4x20</t>
+  </si>
+  <si>
+    <t>parafuso M3xl (l&lt;10)</t>
   </si>
 </sst>
 </file>
@@ -482,7 +494,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -778,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4442A1-F99D-40F7-B3FB-0F573F96FE29}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,15 +1394,15 @@
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
@@ -1401,24 +1413,24 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" s="2">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B34" s="2">
         <v>4</v>
@@ -1430,12 +1442,12 @@
         <v>11</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2">
         <v>3</v>
@@ -1447,11 +1459,51 @@
         <v>11</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>